<commit_message>
feat(App): apply rates first version
</commit_message>
<xml_diff>
--- a/examples/xero/barney-stinson.xlsx
+++ b/examples/xero/barney-stinson.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orozcoj/workspace-personal/correct-hours/examples/xero/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899FE043-0507-954A-920F-2F80C7DD01EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6FF79A-B68E-DF47-8D8C-C6A4B6AB2B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -155,15 +155,15 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
@@ -509,7 +509,7 @@
   <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -533,102 +533,102 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
     </row>
     <row r="2" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
     </row>
     <row r="5" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="N5" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="4">
+      <c r="A6" s="1">
         <v>44185</v>
       </c>
       <c r="B6" t="s">
@@ -672,7 +672,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="4">
+      <c r="A7" s="1">
         <v>44185</v>
       </c>
       <c r="B7" t="s">
@@ -716,7 +716,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="4">
+      <c r="A8" s="1">
         <v>44185</v>
       </c>
       <c r="B8" t="s">
@@ -760,7 +760,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="4">
+      <c r="A9" s="1">
         <v>44213</v>
       </c>
       <c r="B9" t="s">
@@ -804,7 +804,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="4">
+      <c r="A10" s="1">
         <v>44220</v>
       </c>
       <c r="B10" t="s">
@@ -848,7 +848,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="4">
+      <c r="A11" s="1">
         <v>44227</v>
       </c>
       <c r="B11" t="s">
@@ -892,7 +892,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="4">
+      <c r="A12" s="1">
         <v>44234</v>
       </c>
       <c r="B12" t="s">
@@ -936,7 +936,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="4">
+      <c r="A13" s="1">
         <v>44234</v>
       </c>
       <c r="B13" t="s">
@@ -980,7 +980,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="4">
+      <c r="A14" s="1">
         <v>44241</v>
       </c>
       <c r="B14" t="s">
@@ -1024,7 +1024,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="4">
+      <c r="A15" s="1">
         <v>44255</v>
       </c>
       <c r="B15" t="s">
@@ -1068,7 +1068,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="4">
+      <c r="A16" s="1">
         <v>44255</v>
       </c>
       <c r="B16" t="s">
@@ -1112,7 +1112,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="4">
+      <c r="A17" s="1">
         <v>44255</v>
       </c>
       <c r="B17" t="s">
@@ -1156,7 +1156,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="4">
+      <c r="A18" s="1">
         <v>44262</v>
       </c>
       <c r="B18" t="s">
@@ -1200,7 +1200,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="4">
+      <c r="A19" s="1">
         <v>44269</v>
       </c>
       <c r="B19" t="s">
@@ -1244,7 +1244,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="4">
+      <c r="A20" s="1">
         <v>44269</v>
       </c>
       <c r="B20" t="s">
@@ -1288,7 +1288,7 @@
       </c>
     </row>
     <row r="21" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="4">
+      <c r="A21" s="1">
         <v>44269</v>
       </c>
       <c r="B21" t="s">
@@ -1332,7 +1332,7 @@
       </c>
     </row>
     <row r="22" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="4">
+      <c r="A22" s="1">
         <v>44276</v>
       </c>
       <c r="B22" t="s">
@@ -1376,7 +1376,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="4">
+      <c r="A23" s="1">
         <v>44276</v>
       </c>
       <c r="B23" t="s">
@@ -1420,7 +1420,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="4">
+      <c r="A24" s="1">
         <v>44276</v>
       </c>
       <c r="B24" t="s">
@@ -1464,7 +1464,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="4">
+      <c r="A25" s="1">
         <v>44283</v>
       </c>
       <c r="B25" t="s">
@@ -1508,7 +1508,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="4">
+      <c r="A26" s="1">
         <v>44283</v>
       </c>
       <c r="B26" t="s">
@@ -1552,7 +1552,7 @@
       </c>
     </row>
     <row r="27" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="4">
+      <c r="A27" s="1">
         <v>44283</v>
       </c>
       <c r="B27" t="s">
@@ -1596,7 +1596,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="4">
+      <c r="A28" s="1">
         <v>44290</v>
       </c>
       <c r="B28" t="s">
@@ -1640,7 +1640,7 @@
       </c>
     </row>
     <row r="29" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="4">
+      <c r="A29" s="1">
         <v>44290</v>
       </c>
       <c r="B29" t="s">
@@ -1684,7 +1684,7 @@
       </c>
     </row>
     <row r="30" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="4">
+      <c r="A30" s="1">
         <v>44304</v>
       </c>
       <c r="B30" t="s">
@@ -1728,7 +1728,7 @@
       </c>
     </row>
     <row r="31" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="4">
+      <c r="A31" s="1">
         <v>44311</v>
       </c>
       <c r="B31" t="s">
@@ -1772,7 +1772,7 @@
       </c>
     </row>
     <row r="32" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="4">
+      <c r="A32" s="1">
         <v>44311</v>
       </c>
       <c r="B32" t="s">
@@ -1816,7 +1816,7 @@
       </c>
     </row>
     <row r="33" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="4">
+      <c r="A33" s="1">
         <v>44318</v>
       </c>
       <c r="B33" t="s">
@@ -1860,7 +1860,7 @@
       </c>
     </row>
     <row r="34" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="4">
+      <c r="A34" s="1">
         <v>44325</v>
       </c>
       <c r="B34" t="s">
@@ -1904,7 +1904,7 @@
       </c>
     </row>
     <row r="35" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="4">
+      <c r="A35" s="1">
         <v>44325</v>
       </c>
       <c r="B35" t="s">
@@ -1948,7 +1948,7 @@
       </c>
     </row>
     <row r="36" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="4">
+      <c r="A36" s="1">
         <v>44332</v>
       </c>
       <c r="B36" t="s">
@@ -1992,7 +1992,7 @@
       </c>
     </row>
     <row r="37" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="4">
+      <c r="A37" s="1">
         <v>44339</v>
       </c>
       <c r="B37" t="s">
@@ -2036,7 +2036,7 @@
       </c>
     </row>
     <row r="38" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="4">
+      <c r="A38" s="1">
         <v>44339</v>
       </c>
       <c r="B38" t="s">
@@ -2080,7 +2080,7 @@
       </c>
     </row>
     <row r="39" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="4">
+      <c r="A39" s="1">
         <v>44339</v>
       </c>
       <c r="B39" t="s">
@@ -2124,7 +2124,7 @@
       </c>
     </row>
     <row r="40" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="4">
+      <c r="A40" s="1">
         <v>44353</v>
       </c>
       <c r="B40" t="s">
@@ -2168,7 +2168,7 @@
       </c>
     </row>
     <row r="41" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="4">
+      <c r="A41" s="1">
         <v>44353</v>
       </c>
       <c r="B41" t="s">
@@ -2212,7 +2212,7 @@
       </c>
     </row>
     <row r="42" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="4">
+      <c r="A42" s="1">
         <v>44360</v>
       </c>
       <c r="B42" t="s">
@@ -2256,7 +2256,7 @@
       </c>
     </row>
     <row r="43" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="4">
+      <c r="A43" s="1">
         <v>44367</v>
       </c>
       <c r="B43" t="s">
@@ -2300,7 +2300,7 @@
       </c>
     </row>
     <row r="44" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="4">
+      <c r="A44" s="1">
         <v>44374</v>
       </c>
       <c r="B44" t="s">
@@ -2344,7 +2344,7 @@
       </c>
     </row>
     <row r="45" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="4">
+      <c r="A45" s="1">
         <v>44374</v>
       </c>
       <c r="B45" t="s">
@@ -2388,7 +2388,7 @@
       </c>
     </row>
     <row r="46" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="4">
+      <c r="A46" s="1">
         <v>44374</v>
       </c>
       <c r="B46" t="s">
@@ -2432,7 +2432,7 @@
       </c>
     </row>
     <row r="47" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="4">
+      <c r="A47" s="1">
         <v>44381</v>
       </c>
       <c r="B47" t="s">
@@ -2476,7 +2476,7 @@
       </c>
     </row>
     <row r="48" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="4">
+      <c r="A48" s="1">
         <v>44381</v>
       </c>
       <c r="B48" t="s">
@@ -2520,7 +2520,7 @@
       </c>
     </row>
     <row r="49" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="4">
+      <c r="A49" s="1">
         <v>44381</v>
       </c>
       <c r="B49" t="s">

</xml_diff>